<commit_message>
qiu add machine base info
</commit_message>
<xml_diff>
--- a/doc/表设计.xlsx
+++ b/doc/表设计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="关键信息表" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="370">
   <si>
     <t>S/N号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -303,10 +303,6 @@
   </si>
   <si>
     <t>目标对象</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>originObject</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1498,6 +1494,22 @@
   </si>
   <si>
     <t>特殊标记信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>originObject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否可以删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>true或false</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2086,8 +2098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2107,15 +2119,15 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -2202,7 +2214,7 @@
         <v>55</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>57</v>
@@ -2239,10 +2251,10 @@
         <v>60</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="M6" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
@@ -2253,7 +2265,7 @@
         <v>46</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>14</v>
@@ -2262,7 +2274,7 @@
         <v>29</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>61</v>
@@ -2274,7 +2286,7 @@
         <v>63</v>
       </c>
       <c r="M7" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
@@ -2303,7 +2315,7 @@
         <v>66</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M8" s="28" t="s">
         <v>40</v>
@@ -2311,13 +2323,13 @@
     </row>
     <row r="9" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>99</v>
-      </c>
       <c r="D9" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>15</v>
@@ -2329,13 +2341,13 @@
         <v>69</v>
       </c>
       <c r="J9" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="K9" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="K9" s="7" t="s">
-        <v>72</v>
-      </c>
       <c r="L9" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M9" s="28" t="s">
         <v>40</v>
@@ -2361,13 +2373,13 @@
         <v>70</v>
       </c>
       <c r="J10" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="K10" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="L10" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M10" s="28" t="s">
         <v>40</v>
@@ -2390,7 +2402,7 @@
         <v>29</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>67</v>
@@ -2402,7 +2414,7 @@
         <v>23</v>
       </c>
       <c r="M11" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
@@ -2416,19 +2428,19 @@
         <v>39</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F12" s="28" t="s">
         <v>30</v>
       </c>
       <c r="I12" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="K12" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>26</v>
@@ -2454,13 +2466,13 @@
         <v>30</v>
       </c>
       <c r="I13" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K13" s="8" t="s">
         <v>348</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>349</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>31</v>
@@ -2503,13 +2515,13 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>348</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>349</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>31</v>
@@ -2537,12 +2549,12 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I18" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I19" s="16" t="s">
         <v>5</v>
@@ -2577,19 +2589,19 @@
         <v>27</v>
       </c>
       <c r="I20" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="K20" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="J20" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="K20" s="7" t="s">
+      <c r="L20" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="M20" s="28" t="s">
         <v>133</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="M20" s="28" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
@@ -2600,7 +2612,7 @@
         <v>42</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>44</v>
@@ -2609,16 +2621,16 @@
         <v>28</v>
       </c>
       <c r="I21" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="J21" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="K21" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="K21" s="7" t="s">
-        <v>138</v>
-      </c>
       <c r="L21" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M21" s="28"/>
     </row>
@@ -2639,13 +2651,13 @@
         <v>28</v>
       </c>
       <c r="I22" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="J22" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="K22" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="L22" s="8"/>
       <c r="M22" s="28"/>
@@ -2658,69 +2670,69 @@
         <v>45</v>
       </c>
       <c r="D23" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>102</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>103</v>
       </c>
       <c r="F23" s="28" t="s">
         <v>29</v>
       </c>
       <c r="I23" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="J23" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="J23" s="7" t="s">
-        <v>143</v>
-      </c>
       <c r="K23" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L23" s="8"/>
       <c r="M23" s="28"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="8" t="s">
+      <c r="F24" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="F24" s="28" t="s">
-        <v>89</v>
-      </c>
       <c r="I24" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L24" s="13"/>
       <c r="M24" s="37"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C25" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="E25" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="F25" s="28" t="s">
         <v>96</v>
-      </c>
-      <c r="F25" s="28" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
@@ -2731,7 +2743,7 @@
         <v>46</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>14</v>
@@ -2740,18 +2752,18 @@
         <v>29</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="27" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>47</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>15</v>
@@ -2777,13 +2789,13 @@
     </row>
     <row r="28" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="D28" s="8" t="s">
         <v>99</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>100</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>15</v>
@@ -2792,69 +2804,69 @@
         <v>29</v>
       </c>
       <c r="I28" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="J28" s="5" t="s">
-        <v>152</v>
-      </c>
       <c r="K28" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L28" s="32"/>
       <c r="M28" s="36"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>106</v>
-      </c>
       <c r="E29" s="8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F29" s="28" t="s">
         <v>29</v>
       </c>
       <c r="I29" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="J29" s="7" t="s">
         <v>364</v>
       </c>
-      <c r="J29" s="7" t="s">
+      <c r="K29" s="7" t="s">
         <v>365</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>366</v>
       </c>
       <c r="L29" s="8"/>
       <c r="M29" s="28"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="D30" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="E30" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="F30" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="I30" s="11" t="s">
         <v>362</v>
       </c>
-      <c r="F30" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="I30" s="11" t="s">
-        <v>363</v>
-      </c>
       <c r="J30" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L30" s="13"/>
       <c r="M30" s="37"/>
@@ -2870,7 +2882,7 @@
         <v>39</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F31" s="28" t="s">
         <v>28</v>
@@ -2910,18 +2922,18 @@
         <v>28</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>348</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>349</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>31</v>
@@ -2962,19 +2974,19 @@
         <v>28</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J35" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="K35" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>156</v>
       </c>
       <c r="L35" s="26" t="s">
         <v>44</v>
       </c>
       <c r="M35" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.2">
@@ -3003,24 +3015,24 @@
         <v>60</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="M37" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I38" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="J38" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="J38" s="7" t="s">
-        <v>159</v>
-      </c>
       <c r="K38" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L38" s="8"/>
       <c r="M38" s="28"/>
@@ -3042,197 +3054,197 @@
         <v>27</v>
       </c>
       <c r="I39" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="J39" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="J39" s="7" t="s">
+      <c r="K39" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="K39" s="7" t="s">
+      <c r="L39" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="L39" s="8" t="s">
-        <v>166</v>
       </c>
       <c r="M39" s="28"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D40" s="32" t="s">
         <v>171</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D40" s="32" t="s">
-        <v>172</v>
       </c>
       <c r="E40" s="26" t="s">
         <v>44</v>
       </c>
       <c r="F40" s="36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I40" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="J40" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J40" s="7" t="s">
+      <c r="K40" s="7" t="s">
         <v>168</v>
-      </c>
-      <c r="K40" s="7" t="s">
-        <v>169</v>
       </c>
       <c r="L40" s="8" t="s">
         <v>15</v>
       </c>
       <c r="M40" s="28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="28"/>
       <c r="I41" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="J41" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="J41" s="7" t="s">
+      <c r="K41" s="7" t="s">
         <v>328</v>
-      </c>
-      <c r="K41" s="7" t="s">
-        <v>329</v>
       </c>
       <c r="L41" s="8"/>
       <c r="M41" s="28"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="D42" s="8" t="s">
         <v>178</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>179</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="28"/>
       <c r="I42" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="J42" s="7" t="s">
         <v>330</v>
       </c>
-      <c r="J42" s="7" t="s">
+      <c r="K42" s="7" t="s">
         <v>331</v>
-      </c>
-      <c r="K42" s="7" t="s">
-        <v>332</v>
       </c>
       <c r="L42" s="8"/>
       <c r="M42" s="28"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="D43" s="8" t="s">
         <v>181</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>182</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="28"/>
       <c r="I43" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="J43" s="7" t="s">
         <v>350</v>
       </c>
-      <c r="J43" s="7" t="s">
+      <c r="K43" s="7" t="s">
         <v>351</v>
-      </c>
-      <c r="K43" s="7" t="s">
-        <v>352</v>
       </c>
       <c r="L43" s="8"/>
       <c r="M43" s="28"/>
     </row>
     <row r="44" spans="2:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B44" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="C44" s="7" t="s">
-        <v>184</v>
-      </c>
       <c r="D44" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="E44" s="8" t="s">
         <v>188</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>189</v>
       </c>
       <c r="F44" s="28"/>
       <c r="I44" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="J44" s="7" t="s">
         <v>334</v>
       </c>
-      <c r="J44" s="7" t="s">
-        <v>335</v>
-      </c>
       <c r="K44" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="L44" s="8"/>
       <c r="M44" s="28"/>
     </row>
     <row r="45" spans="2:13" ht="99.75" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="D45" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="D45" s="8" t="s">
-        <v>187</v>
-      </c>
       <c r="E45" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F45" s="28"/>
       <c r="I45" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="J45" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="J45" s="7" t="s">
-        <v>337</v>
-      </c>
       <c r="K45" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="L45" s="8"/>
       <c r="M45" s="28"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B46" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="C46" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="D46" s="8" t="s">
+      <c r="E46" s="7" t="s">
         <v>192</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>193</v>
       </c>
       <c r="F46" s="28"/>
       <c r="I46" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="J46" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="J46" s="7" t="s">
-        <v>354</v>
-      </c>
       <c r="K46" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L46" s="10" t="s">
         <v>31</v>
@@ -3243,16 +3255,16 @@
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="D47" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="E47" s="8" t="s">
         <v>196</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>197</v>
       </c>
       <c r="F47" s="28"/>
       <c r="I47" s="11" t="s">
@@ -3307,13 +3319,13 @@
     </row>
     <row r="50" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B50" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D50" s="8" t="s">
         <v>348</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>349</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>31</v>
@@ -3322,10 +3334,10 @@
         <v>32</v>
       </c>
       <c r="I50" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="J50" s="3" t="s">
         <v>324</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>325</v>
       </c>
       <c r="K50" s="3"/>
       <c r="L50" s="1"/>
@@ -3368,13 +3380,13 @@
       <c r="C52" s="3"/>
       <c r="F52" s="3"/>
       <c r="I52" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="K52" s="32" t="s">
         <v>111</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="K52" s="32" t="s">
-        <v>112</v>
       </c>
       <c r="L52" s="26" t="s">
         <v>44</v>
@@ -3385,19 +3397,19 @@
     </row>
     <row r="53" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I53" s="34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J53" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K53" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L53" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M53" s="35"/>
     </row>
@@ -3418,7 +3430,7 @@
         <v>27</v>
       </c>
       <c r="I54" s="34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J54" s="7" t="s">
         <v>56</v>
@@ -3446,19 +3458,19 @@
         <v>36</v>
       </c>
       <c r="I55" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="J55" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="J55" s="8" t="s">
+      <c r="K55" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="K55" s="8" t="s">
+      <c r="L55" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="M55" s="35" t="s">
         <v>121</v>
-      </c>
-      <c r="L55" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="M55" s="35" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="56" spans="2:13" ht="42.75" x14ac:dyDescent="0.2">
@@ -3469,7 +3481,7 @@
         <v>45</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>13</v>
@@ -3478,16 +3490,16 @@
         <v>29</v>
       </c>
       <c r="I56" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="J56" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="J56" s="8" t="s">
+      <c r="K56" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="K56" s="8" t="s">
+      <c r="L56" s="10" t="s">
         <v>129</v>
-      </c>
-      <c r="L56" s="10" t="s">
-        <v>130</v>
       </c>
       <c r="M56" s="35"/>
     </row>
@@ -3499,7 +3511,7 @@
         <v>46</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>14</v>
@@ -3508,16 +3520,16 @@
         <v>29</v>
       </c>
       <c r="I57" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="J57" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="J57" s="8" t="s">
+      <c r="K57" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="K57" s="8" t="s">
+      <c r="L57" s="10" t="s">
         <v>125</v>
-      </c>
-      <c r="L57" s="10" t="s">
-        <v>126</v>
       </c>
       <c r="M57" s="35"/>
     </row>
@@ -3555,13 +3567,13 @@
     </row>
     <row r="59" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B59" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C59" s="7" t="s">
-        <v>99</v>
-      </c>
       <c r="D59" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>15</v>
@@ -3587,13 +3599,13 @@
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B60" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="D60" s="8" t="s">
         <v>313</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>314</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>18</v>
@@ -3602,13 +3614,13 @@
         <v>29</v>
       </c>
       <c r="I60" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="J60" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K60" s="8" t="s">
         <v>348</v>
-      </c>
-      <c r="J60" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="K60" s="8" t="s">
-        <v>349</v>
       </c>
       <c r="L60" s="8" t="s">
         <v>31</v>
@@ -3619,16 +3631,16 @@
     </row>
     <row r="61" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B61" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>49</v>
       </c>
       <c r="D61" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="E61" s="8" t="s">
         <v>316</v>
-      </c>
-      <c r="E61" s="8" t="s">
-        <v>317</v>
       </c>
       <c r="F61" s="28" t="s">
         <v>29</v>
@@ -3651,16 +3663,16 @@
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B62" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="C62" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="D62" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="E62" s="8" t="s">
         <v>322</v>
-      </c>
-      <c r="E62" s="8" t="s">
-        <v>323</v>
       </c>
       <c r="F62" s="28"/>
     </row>
@@ -3675,7 +3687,7 @@
         <v>39</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F63" s="28" t="s">
         <v>30</v>
@@ -3698,7 +3710,7 @@
         <v>30</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.2">
@@ -3735,13 +3747,13 @@
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B66" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D66" s="8" t="s">
         <v>348</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D66" s="8" t="s">
-        <v>349</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>31</v>
@@ -3750,13 +3762,13 @@
         <v>32</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J66" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="K66" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="K66" s="5" t="s">
-        <v>200</v>
       </c>
       <c r="L66" s="26" t="s">
         <v>44</v>
@@ -3782,93 +3794,93 @@
         <v>36</v>
       </c>
       <c r="I67" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="J67" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="K67" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="J67" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="K67" s="7" t="s">
+      <c r="L67" s="8" t="s">
         <v>202</v>
-      </c>
-      <c r="L67" s="8" t="s">
-        <v>203</v>
       </c>
       <c r="M67" s="28"/>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I68" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="J68" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="K68" s="7" t="s">
         <v>204</v>
-      </c>
-      <c r="J68" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="K68" s="7" t="s">
-        <v>205</v>
       </c>
       <c r="L68" s="8"/>
       <c r="M68" s="28"/>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I69" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J69" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K69" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L69" s="8"/>
       <c r="M69" s="28"/>
     </row>
     <row r="70" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I70" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="J70" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="K70" s="7" t="s">
         <v>209</v>
-      </c>
-      <c r="J70" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="K70" s="7" t="s">
-        <v>210</v>
       </c>
       <c r="L70" s="8"/>
       <c r="M70" s="28"/>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I71" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="J71" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="K71" s="7" t="s">
         <v>211</v>
-      </c>
-      <c r="J71" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="K71" s="7" t="s">
-        <v>212</v>
       </c>
       <c r="L71" s="8"/>
       <c r="M71" s="28"/>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I72" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="J72" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="J72" s="7" t="s">
+      <c r="K72" s="7" t="s">
         <v>215</v>
-      </c>
-      <c r="K72" s="7" t="s">
-        <v>216</v>
       </c>
       <c r="L72" s="8"/>
       <c r="M72" s="28"/>
     </row>
     <row r="73" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I73" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="J73" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="J73" s="12" t="s">
+      <c r="K73" s="12" t="s">
         <v>301</v>
-      </c>
-      <c r="K73" s="12" t="s">
-        <v>302</v>
       </c>
       <c r="L73" s="13"/>
       <c r="M73" s="37"/>
@@ -3884,8 +3896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3906,15 +3918,15 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -3951,192 +3963,192 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D6" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="E6" s="32" t="s">
         <v>222</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="F6" s="39" t="s">
         <v>223</v>
       </c>
-      <c r="F6" s="39" t="s">
-        <v>224</v>
-      </c>
       <c r="I6" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="K6" s="32" t="s">
         <v>261</v>
-      </c>
-      <c r="K6" s="32" t="s">
-        <v>262</v>
       </c>
       <c r="L6" s="5"/>
       <c r="M6" s="36"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>227</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>228</v>
       </c>
       <c r="F7" s="40"/>
       <c r="I7" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="K7" s="8" t="s">
         <v>264</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>265</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="28"/>
     </row>
     <row r="8" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B8" s="34" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="40"/>
       <c r="I8" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>266</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>267</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="28"/>
     </row>
     <row r="9" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B9" s="41" t="s">
+        <v>339</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>340</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>341</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="42"/>
       <c r="I9" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="J9" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="K9" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="K9" s="8" t="s">
-        <v>271</v>
-      </c>
       <c r="L9" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="M9" s="28"/>
     </row>
     <row r="10" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="I10" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="J10" s="7" t="s">
-        <v>273</v>
-      </c>
       <c r="K10" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L10" s="7"/>
       <c r="M10" s="28"/>
     </row>
     <row r="11" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B11" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="D11" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="E11" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="E11" s="38" t="s">
-        <v>232</v>
-      </c>
       <c r="I11" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="J11" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="J11" s="7" t="s">
-        <v>275</v>
-      </c>
       <c r="K11" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L11" s="7"/>
       <c r="M11" s="28"/>
     </row>
     <row r="12" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B12" s="31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C12" s="32" t="s">
+        <v>302</v>
+      </c>
+      <c r="D12" s="32" t="s">
         <v>303</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="E12" s="39" t="s">
         <v>304</v>
       </c>
-      <c r="E12" s="39" t="s">
-        <v>305</v>
-      </c>
       <c r="I12" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="K12" s="8" t="s">
         <v>359</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>360</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="28"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="41" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C13" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>306</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="E13" s="42" t="s">
         <v>307</v>
       </c>
-      <c r="E13" s="42" t="s">
-        <v>308</v>
-      </c>
       <c r="I13" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="J13" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="K13" s="13" t="s">
         <v>279</v>
-      </c>
-      <c r="K13" s="13" t="s">
-        <v>280</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="37"/>
@@ -4150,7 +4162,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="44" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="43"/>
@@ -4164,7 +4176,7 @@
       <c r="E16" s="43"/>
       <c r="F16" s="43"/>
       <c r="I16" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.2">
@@ -4186,29 +4198,29 @@
     </row>
     <row r="18" spans="2:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="I18" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K18" s="32" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="36"/>
     </row>
     <row r="19" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I19" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="K19" s="8" t="s">
         <v>346</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>347</v>
       </c>
       <c r="L19" s="7"/>
       <c r="M19" s="28"/>
@@ -4230,150 +4242,161 @@
         <v>27</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L20" s="7"/>
       <c r="M20" s="28"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" s="31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E21" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="F21" s="39" t="s">
         <v>223</v>
       </c>
-      <c r="F21" s="39" t="s">
-        <v>224</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="K21" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="L21" s="12"/>
-      <c r="M21" s="37"/>
+      <c r="I21" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="L21" s="7"/>
+      <c r="M21" s="28"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" s="34" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C22" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>228</v>
-      </c>
       <c r="F22" s="40"/>
+      <c r="I22" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="L22" s="12"/>
+      <c r="M22" s="37"/>
     </row>
     <row r="23" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B23" s="34" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="40"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" s="41" t="s">
+        <v>341</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D24" s="13" t="s">
         <v>342</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>343</v>
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="42"/>
       <c r="I24" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K24" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="L24" s="17" t="s">
         <v>288</v>
       </c>
-      <c r="L24" s="17" t="s">
+      <c r="M24" s="24" t="s">
         <v>289</v>
-      </c>
-      <c r="M24" s="24" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I25" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J25" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="K25" s="32" t="s">
         <v>293</v>
       </c>
-      <c r="K25" s="32" t="s">
+      <c r="L25" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="M25" s="36" t="s">
         <v>295</v>
-      </c>
-      <c r="M25" s="36" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I26" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J26" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="K26" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="K26" s="8" t="s">
-        <v>294</v>
-      </c>
       <c r="L26" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="M26" s="28" t="s">
         <v>297</v>
-      </c>
-      <c r="M26" s="28" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="C27" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="D27" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="E27" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="E27" s="38" t="s">
-        <v>232</v>
-      </c>
       <c r="I27" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J27" s="12"/>
       <c r="K27" s="13"/>
@@ -4382,30 +4405,30 @@
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B28" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C28" s="32" t="s">
+        <v>240</v>
+      </c>
+      <c r="D28" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="D28" s="32" t="s">
+      <c r="E28" s="39" t="s">
         <v>242</v>
-      </c>
-      <c r="E28" s="39" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B29" s="41" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C29" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="E29" s="42" t="s">
         <v>244</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="E29" s="42" t="s">
-        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
qiu addmachine select data
</commit_message>
<xml_diff>
--- a/doc/表设计.xlsx
+++ b/doc/表设计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="关键信息表" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="373">
   <si>
     <t>S/N号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -342,10 +342,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>createTime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>新增这条记录的时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -394,10 +390,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>fixedNumber</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>公司级固定资产编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1182,10 +1174,6 @@
   </si>
   <si>
     <t>S0001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设备归属表(ascription)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1510,6 +1498,30 @@
   </si>
   <si>
     <t>true或false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所属类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给选项自行设置的标签</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>createTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备归属表(ascription)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixedNumber</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2098,8 +2110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2119,15 +2131,15 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>291</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -2214,7 +2226,7 @@
         <v>55</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>57</v>
@@ -2251,7 +2263,7 @@
         <v>60</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="M6" s="28" t="s">
         <v>76</v>
@@ -2265,7 +2277,7 @@
         <v>46</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>14</v>
@@ -2274,7 +2286,7 @@
         <v>29</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>61</v>
@@ -2323,13 +2335,13 @@
     </row>
     <row r="9" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>15</v>
@@ -2341,13 +2353,13 @@
         <v>69</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>71</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M9" s="28" t="s">
         <v>40</v>
@@ -2379,7 +2391,7 @@
         <v>73</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M10" s="28" t="s">
         <v>40</v>
@@ -2414,7 +2426,7 @@
         <v>23</v>
       </c>
       <c r="M11" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
@@ -2428,7 +2440,7 @@
         <v>39</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F12" s="28" t="s">
         <v>30</v>
@@ -2437,10 +2449,10 @@
         <v>79</v>
       </c>
       <c r="J12" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="K12" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>81</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>26</v>
@@ -2466,13 +2478,13 @@
         <v>30</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>31</v>
@@ -2515,13 +2527,13 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>31</v>
@@ -2549,12 +2561,12 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I18" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I19" s="16" t="s">
         <v>5</v>
@@ -2589,19 +2601,19 @@
         <v>27</v>
       </c>
       <c r="I20" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="M20" s="28" t="s">
         <v>131</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="M20" s="28" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
@@ -2612,7 +2624,7 @@
         <v>42</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>44</v>
@@ -2621,16 +2633,16 @@
         <v>28</v>
       </c>
       <c r="I21" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="K21" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="J21" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>137</v>
-      </c>
       <c r="L21" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M21" s="28"/>
     </row>
@@ -2651,13 +2663,13 @@
         <v>28</v>
       </c>
       <c r="I22" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="K22" s="7" t="s">
         <v>138</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>140</v>
       </c>
       <c r="L22" s="8"/>
       <c r="M22" s="28"/>
@@ -2670,69 +2682,69 @@
         <v>45</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F23" s="28" t="s">
         <v>29</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L23" s="8"/>
       <c r="M23" s="28"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" s="8" t="s">
+      <c r="F24" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="F24" s="28" t="s">
-        <v>88</v>
-      </c>
       <c r="I24" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="K24" s="12" t="s">
         <v>144</v>
-      </c>
-      <c r="J24" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="K24" s="12" t="s">
-        <v>146</v>
       </c>
       <c r="L24" s="13"/>
       <c r="M24" s="37"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="F25" s="28" t="s">
         <v>94</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F25" s="28" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
@@ -2743,7 +2755,7 @@
         <v>46</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>14</v>
@@ -2752,18 +2764,18 @@
         <v>29</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>47</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>15</v>
@@ -2789,13 +2801,13 @@
     </row>
     <row r="28" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>15</v>
@@ -2804,69 +2816,69 @@
         <v>29</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L28" s="32"/>
       <c r="M28" s="36"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>105</v>
-      </c>
       <c r="E29" s="8" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F29" s="28" t="s">
         <v>29</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="L29" s="8"/>
       <c r="M29" s="28"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="E30" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F30" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>361</v>
-      </c>
-      <c r="F30" s="28" t="s">
-        <v>109</v>
-      </c>
       <c r="I30" s="11" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L30" s="13"/>
       <c r="M30" s="37"/>
@@ -2922,18 +2934,18 @@
         <v>28</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>31</v>
@@ -2974,19 +2986,19 @@
         <v>28</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="L35" s="26" t="s">
         <v>44</v>
       </c>
       <c r="M35" s="36" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.2">
@@ -3015,7 +3027,7 @@
         <v>60</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="M37" s="28" t="s">
         <v>76</v>
@@ -3023,16 +3035,16 @@
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J38" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="K38" s="7" t="s">
         <v>158</v>
-      </c>
-      <c r="K38" s="7" t="s">
-        <v>160</v>
       </c>
       <c r="L38" s="8"/>
       <c r="M38" s="28"/>
@@ -3054,197 +3066,197 @@
         <v>27</v>
       </c>
       <c r="I39" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="J39" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="K39" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="J39" s="7" t="s">
+      <c r="L39" s="8" t="s">
         <v>163</v>
-      </c>
-      <c r="K39" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="L39" s="8" t="s">
-        <v>165</v>
       </c>
       <c r="M39" s="28"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D40" s="32" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E40" s="26" t="s">
         <v>44</v>
       </c>
       <c r="F40" s="36" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I40" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="K40" s="7" t="s">
         <v>166</v>
-      </c>
-      <c r="J40" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="K40" s="7" t="s">
-        <v>168</v>
       </c>
       <c r="L40" s="8" t="s">
         <v>15</v>
       </c>
       <c r="M40" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B41" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C41" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>175</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="28"/>
       <c r="I41" s="6" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="K41" s="7" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="L41" s="8"/>
       <c r="M41" s="28"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>176</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>178</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="28"/>
       <c r="I42" s="6" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="L42" s="8"/>
       <c r="M42" s="28"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B43" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>181</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="28"/>
       <c r="I43" s="6" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="L43" s="8"/>
       <c r="M43" s="28"/>
     </row>
     <row r="44" spans="2:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B44" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F44" s="28"/>
       <c r="I44" s="6" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="J44" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="K44" s="7" t="s">
         <v>334</v>
-      </c>
-      <c r="K44" s="7" t="s">
-        <v>337</v>
       </c>
       <c r="L44" s="8"/>
       <c r="M44" s="28"/>
     </row>
     <row r="45" spans="2:13" ht="99.75" x14ac:dyDescent="0.2">
       <c r="B45" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="C45" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>186</v>
-      </c>
       <c r="E45" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F45" s="28"/>
       <c r="I45" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="K45" s="7" t="s">
         <v>335</v>
-      </c>
-      <c r="J45" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="K45" s="7" t="s">
-        <v>338</v>
       </c>
       <c r="L45" s="8"/>
       <c r="M45" s="28"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B46" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E46" s="7" t="s">
         <v>190</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>192</v>
       </c>
       <c r="F46" s="28"/>
       <c r="I46" s="6" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="L46" s="10" t="s">
         <v>31</v>
@@ -3255,16 +3267,16 @@
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B47" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="E47" s="8" t="s">
         <v>194</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>196</v>
       </c>
       <c r="F47" s="28"/>
       <c r="I47" s="11" t="s">
@@ -3319,13 +3331,13 @@
     </row>
     <row r="50" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B50" s="6" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>31</v>
@@ -3334,10 +3346,10 @@
         <v>32</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="K50" s="3"/>
       <c r="L50" s="1"/>
@@ -3380,13 +3392,13 @@
       <c r="C52" s="3"/>
       <c r="F52" s="3"/>
       <c r="I52" s="31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K52" s="32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L52" s="26" t="s">
         <v>44</v>
@@ -3397,19 +3409,19 @@
     </row>
     <row r="53" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="I53" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="J53" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="J53" s="7" t="s">
-        <v>117</v>
-      </c>
       <c r="K53" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="L53" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="L53" s="10" t="s">
-        <v>114</v>
       </c>
       <c r="M53" s="35"/>
     </row>
@@ -3430,7 +3442,7 @@
         <v>27</v>
       </c>
       <c r="I54" s="34" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J54" s="7" t="s">
         <v>56</v>
@@ -3458,19 +3470,19 @@
         <v>36</v>
       </c>
       <c r="I55" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K55" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="J55" s="8" t="s">
+      <c r="L55" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="M55" s="35" t="s">
         <v>119</v>
-      </c>
-      <c r="K55" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="L55" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="M55" s="35" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="56" spans="2:13" ht="42.75" x14ac:dyDescent="0.2">
@@ -3481,7 +3493,7 @@
         <v>45</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>13</v>
@@ -3490,16 +3502,16 @@
         <v>29</v>
       </c>
       <c r="I56" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="J56" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="K56" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="J56" s="8" t="s">
+      <c r="L56" s="10" t="s">
         <v>127</v>
-      </c>
-      <c r="K56" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="L56" s="10" t="s">
-        <v>129</v>
       </c>
       <c r="M56" s="35"/>
     </row>
@@ -3511,7 +3523,7 @@
         <v>46</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>14</v>
@@ -3520,16 +3532,16 @@
         <v>29</v>
       </c>
       <c r="I57" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="J57" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="K57" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="J57" s="8" t="s">
+      <c r="L57" s="10" t="s">
         <v>123</v>
-      </c>
-      <c r="K57" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="L57" s="10" t="s">
-        <v>125</v>
       </c>
       <c r="M57" s="35"/>
     </row>
@@ -3567,13 +3579,13 @@
     </row>
     <row r="59" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B59" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>15</v>
@@ -3599,13 +3611,13 @@
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B60" s="6" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>18</v>
@@ -3614,13 +3626,13 @@
         <v>29</v>
       </c>
       <c r="I60" s="6" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="J60" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K60" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="L60" s="8" t="s">
         <v>31</v>
@@ -3631,16 +3643,16 @@
     </row>
     <row r="61" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B61" s="6" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>49</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F61" s="28" t="s">
         <v>29</v>
@@ -3663,16 +3675,16 @@
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B62" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="E62" s="8" t="s">
         <v>319</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="E62" s="8" t="s">
-        <v>322</v>
       </c>
       <c r="F62" s="28"/>
     </row>
@@ -3687,7 +3699,7 @@
         <v>39</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F63" s="28" t="s">
         <v>30</v>
@@ -3710,7 +3722,7 @@
         <v>30</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.2">
@@ -3747,13 +3759,13 @@
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B66" s="6" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>31</v>
@@ -3762,13 +3774,13 @@
         <v>32</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K66" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L66" s="26" t="s">
         <v>44</v>
@@ -3794,93 +3806,93 @@
         <v>36</v>
       </c>
       <c r="I67" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="J67" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="K67" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="L67" s="8" t="s">
         <v>200</v>
-      </c>
-      <c r="J67" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="K67" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="L67" s="8" t="s">
-        <v>202</v>
       </c>
       <c r="M67" s="28"/>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I68" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J68" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K68" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="L68" s="8"/>
       <c r="M68" s="28"/>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I69" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="J69" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="K69" s="7" t="s">
         <v>205</v>
-      </c>
-      <c r="J69" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="K69" s="7" t="s">
-        <v>207</v>
       </c>
       <c r="L69" s="8"/>
       <c r="M69" s="28"/>
     </row>
     <row r="70" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I70" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J70" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K70" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="L70" s="8"/>
       <c r="M70" s="28"/>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I71" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="J71" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="J71" s="7" t="s">
-        <v>212</v>
-      </c>
       <c r="K71" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L71" s="8"/>
       <c r="M71" s="28"/>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I72" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="J72" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="K72" s="7" t="s">
         <v>213</v>
-      </c>
-      <c r="J72" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="K72" s="7" t="s">
-        <v>215</v>
       </c>
       <c r="L72" s="8"/>
       <c r="M72" s="28"/>
     </row>
     <row r="73" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I73" s="11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="J73" s="12" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="K73" s="12" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="L73" s="13"/>
       <c r="M73" s="37"/>
@@ -3896,8 +3908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3918,15 +3930,15 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -3963,192 +3975,192 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="D6" s="32" t="s">
         <v>219</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="E6" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="F6" s="39" t="s">
         <v>221</v>
       </c>
-      <c r="E6" s="32" t="s">
-        <v>222</v>
-      </c>
-      <c r="F6" s="39" t="s">
-        <v>223</v>
-      </c>
       <c r="I6" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="K6" s="32" t="s">
         <v>259</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="K6" s="32" t="s">
-        <v>261</v>
       </c>
       <c r="L6" s="5"/>
       <c r="M6" s="36"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="34" t="s">
+        <v>223</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>225</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>227</v>
       </c>
       <c r="F7" s="40"/>
       <c r="I7" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="K7" s="8" t="s">
         <v>262</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>264</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="28"/>
     </row>
     <row r="8" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B8" s="34" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="40"/>
       <c r="I8" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="28"/>
     </row>
     <row r="9" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B9" s="41" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="42"/>
       <c r="I9" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="K9" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="J9" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>270</v>
-      </c>
       <c r="L9" s="7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M9" s="28"/>
     </row>
     <row r="10" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="I10" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="L10" s="7"/>
       <c r="M10" s="28"/>
     </row>
     <row r="11" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B11" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="D11" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="E11" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="E11" s="38" t="s">
-        <v>231</v>
-      </c>
       <c r="I11" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J11" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="K11" s="8" t="s">
         <v>274</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>276</v>
       </c>
       <c r="L11" s="7"/>
       <c r="M11" s="28"/>
     </row>
     <row r="12" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B12" s="31" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E12" s="39" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="28"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="41" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E13" s="42" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="I13" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="K13" s="13" t="s">
         <v>277</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="K13" s="13" t="s">
-        <v>279</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="37"/>
@@ -4162,7 +4174,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="44" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="43"/>
@@ -4176,7 +4188,7 @@
       <c r="E16" s="43"/>
       <c r="F16" s="43"/>
       <c r="I16" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.2">
@@ -4198,29 +4210,29 @@
     </row>
     <row r="18" spans="2:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="I18" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K18" s="32" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="36"/>
     </row>
     <row r="19" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="L19" s="7"/>
       <c r="M19" s="28"/>
@@ -4242,193 +4254,204 @@
         <v>27</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="L20" s="7"/>
       <c r="M20" s="28"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" s="31" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F21" s="39" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="L21" s="7"/>
       <c r="M21" s="28"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B22" s="34" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F22" s="40"/>
-      <c r="I22" s="11" t="s">
+      <c r="I22" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="J22" s="12" t="s">
+      <c r="J22" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="K22" s="13" t="s">
+      <c r="K22" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="L22" s="12"/>
-      <c r="M22" s="37"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="28"/>
     </row>
     <row r="23" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B23" s="34" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="40"/>
+      <c r="I23" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="L23" s="12"/>
+      <c r="M23" s="37"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" s="41" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="42"/>
-      <c r="I24" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="J24" s="17" t="s">
-        <v>260</v>
-      </c>
-      <c r="K24" s="18" t="s">
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="I25" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="K25" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="M25" s="24" t="s">
         <v>287</v>
       </c>
-      <c r="L24" s="17" t="s">
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="I26" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="M24" s="24" t="s">
+      <c r="J26" s="5" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="I25" s="4" t="s">
+      <c r="K26" s="32" t="s">
         <v>290</v>
       </c>
-      <c r="J25" s="5" t="s">
+      <c r="L26" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="M26" s="36" t="s">
         <v>292</v>
-      </c>
-      <c r="K25" s="32" t="s">
-        <v>293</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="M25" s="36" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="I26" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="K26" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="L26" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="M26" s="28" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="D27" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="E27" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="D27" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="E27" s="38" t="s">
-        <v>231</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>298</v>
-      </c>
-      <c r="J27" s="12"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="37"/>
+      <c r="I27" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="M27" s="28" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B28" s="31" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C28" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="E28" s="39" t="s">
         <v>240</v>
       </c>
-      <c r="D28" s="32" t="s">
-        <v>241</v>
-      </c>
-      <c r="E28" s="39" t="s">
-        <v>242</v>
-      </c>
+      <c r="I28" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="J28" s="12"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="37"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B29" s="41" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merge branches 'master' and 'qiuzhujun' of github.com.sub:jochenshi/asset-activity into qiuzhujun
# Conflicts:
#	doc/表设计.xlsx
</commit_message>
<xml_diff>
--- a/doc/表设计.xlsx
+++ b/doc/表设计.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
-  <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jochenshi/Desktop/Personal/code/asset-activity/doc/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3140" windowWidth="38400" windowHeight="21140"/>
+    <workbookView xWindow="-38400" yWindow="-3135" windowWidth="38400" windowHeight="21135"/>
   </bookViews>
   <sheets>
     <sheet name="关键信息表" sheetId="2" r:id="rId1"/>
@@ -20,18 +15,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="415">
   <si>
     <t>S/N号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1721,11 +1716,23 @@
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>是否被删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否已经被删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2397,25 +2404,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M75"/>
+  <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13.125" customWidth="1"/>
     <col min="2" max="2" width="12" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="2"/>
-    <col min="9" max="9" width="17.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.875" style="2"/>
+    <col min="9" max="9" width="17.375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="22.375" style="2" customWidth="1"/>
     <col min="12" max="12" width="44" style="3" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="2"/>
+    <col min="13" max="13" width="8.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -2525,7 +2532,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
@@ -2558,7 +2565,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
@@ -2590,7 +2597,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
@@ -2622,7 +2629,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>95</v>
       </c>
@@ -2686,7 +2693,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
@@ -2718,7 +2725,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="71.25" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
         <v>38</v>
       </c>
@@ -2831,7 +2838,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
         <v>33</v>
       </c>
@@ -2963,7 +2970,7 @@
       <c r="L22" s="8"/>
       <c r="M22" s="28"/>
     </row>
-    <row r="23" spans="2:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
         <v>2</v>
       </c>
@@ -3056,7 +3063,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
         <v>88</v>
       </c>
@@ -3088,7 +3095,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="2:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
         <v>95</v>
       </c>
@@ -3172,7 +3179,7 @@
       <c r="L30" s="13"/>
       <c r="M30" s="37"/>
     </row>
-    <row r="31" spans="2:13" ht="60" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:13" ht="57" x14ac:dyDescent="0.2">
       <c r="B31" s="6" t="s">
         <v>38</v>
       </c>
@@ -3258,7 +3265,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="2:13" ht="45" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B35" s="11" t="s">
         <v>33</v>
       </c>
@@ -3472,7 +3479,7 @@
       <c r="L43" s="8"/>
       <c r="M43" s="28"/>
     </row>
-    <row r="44" spans="2:13" ht="45" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B44" s="67" t="s">
         <v>175</v>
       </c>
@@ -3498,7 +3505,7 @@
       <c r="L44" s="8"/>
       <c r="M44" s="28"/>
     </row>
-    <row r="45" spans="2:13" ht="105" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:13" ht="99.75" x14ac:dyDescent="0.2">
       <c r="B45" s="67" t="s">
         <v>177</v>
       </c>
@@ -3618,7 +3625,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="2:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B50" s="6" t="s">
         <v>338</v>
       </c>
@@ -3644,7 +3651,7 @@
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
     </row>
-    <row r="51" spans="2:13" ht="45" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B51" s="11" t="s">
         <v>33</v>
       </c>
@@ -3696,7 +3703,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="2:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>301</v>
       </c>
@@ -3742,7 +3749,7 @@
       <c r="L54" s="10"/>
       <c r="M54" s="35"/>
     </row>
-    <row r="55" spans="2:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B55" s="21" t="s">
         <v>41</v>
       </c>
@@ -3774,7 +3781,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="56" spans="2:13" ht="45" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B56" s="6" t="s">
         <v>2</v>
       </c>
@@ -3804,7 +3811,7 @@
       </c>
       <c r="M56" s="35"/>
     </row>
-    <row r="57" spans="2:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B57" s="6" t="s">
         <v>4</v>
       </c>
@@ -3834,7 +3841,7 @@
       </c>
       <c r="M57" s="35"/>
     </row>
-    <row r="58" spans="2:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B58" s="6" t="s">
         <v>9</v>
       </c>
@@ -3864,7 +3871,7 @@
       </c>
       <c r="M58" s="35"/>
     </row>
-    <row r="59" spans="2:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B59" s="6" t="s">
         <v>95</v>
       </c>
@@ -3926,7 +3933,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="2:13" ht="45" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B61" s="6" t="s">
         <v>305</v>
       </c>
@@ -3988,7 +3995,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="2:13" ht="75" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:13" ht="71.25" x14ac:dyDescent="0.2">
       <c r="B63" s="6" t="s">
         <v>38</v>
       </c>
@@ -4004,21 +4011,17 @@
       <c r="F63" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="I63" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="J63" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="K63" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="L63" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="M63" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="I63" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="J63" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="K63" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="L63" s="8"/>
+      <c r="M63" s="28"/>
     </row>
     <row r="64" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B64" s="6" t="s">
@@ -4036,6 +4039,21 @@
       <c r="F64" s="28" t="s">
         <v>30</v>
       </c>
+      <c r="I64" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J64" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="K64" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L64" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="M64" s="15" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B65" s="6" t="s">
@@ -4070,11 +4088,8 @@
       <c r="F66" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="I66" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="67" spans="2:13" ht="45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="2:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B67" s="11" t="s">
         <v>33</v>
       </c>
@@ -4090,131 +4105,136 @@
       <c r="F67" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="I67" s="29" t="s">
+      <c r="I67" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="68" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="I68" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="J67" s="18" t="s">
+      <c r="J68" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="K67" s="18" t="s">
+      <c r="K68" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="L67" s="18" t="s">
+      <c r="L68" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="M67" s="30" t="s">
+      <c r="M68" s="30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="I68" s="4" t="s">
+    <row r="69" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="I69" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="J68" s="5" t="s">
+      <c r="J69" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="K68" s="5" t="s">
+      <c r="K69" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="L68" s="26" t="s">
+      <c r="L69" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="M68" s="33" t="s">
+      <c r="M69" s="33" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="2:13" ht="30" x14ac:dyDescent="0.2">
-      <c r="I69" s="6" t="s">
+    <row r="70" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="I70" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="J69" s="7" t="s">
+      <c r="J70" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="K69" s="7" t="s">
+      <c r="K70" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="L69" s="8" t="s">
+      <c r="L70" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="M69" s="28"/>
-    </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="I70" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="J70" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="K70" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="L70" s="8"/>
       <c r="M70" s="28"/>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I71" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J71" s="7" t="s">
-        <v>154</v>
+        <v>199</v>
       </c>
       <c r="K71" s="7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L71" s="8"/>
       <c r="M71" s="28"/>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I72" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="J72" s="7" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="K72" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L72" s="8"/>
       <c r="M72" s="28"/>
     </row>
     <row r="73" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I73" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J73" s="7" t="s">
-        <v>205</v>
+        <v>151</v>
       </c>
       <c r="K73" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="L73" s="8"/>
       <c r="M73" s="28"/>
     </row>
     <row r="74" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I74" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="J74" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K74" s="7" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="L74" s="8"/>
       <c r="M74" s="28"/>
     </row>
     <row r="75" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="I75" s="11" t="s">
+      <c r="I75" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="J75" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="K75" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="L75" s="8"/>
+      <c r="M75" s="28"/>
+    </row>
+    <row r="76" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="I76" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="J75" s="12" t="s">
+      <c r="J76" s="12" t="s">
         <v>291</v>
       </c>
-      <c r="K75" s="12" t="s">
+      <c r="K76" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="L75" s="13"/>
-      <c r="M75" s="37"/>
+      <c r="L76" s="13"/>
+      <c r="M76" s="37"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4231,20 +4251,20 @@
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="3"/>
-    <col min="2" max="2" width="10.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" style="3" customWidth="1"/>
-    <col min="6" max="8" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="8.875" style="3"/>
+    <col min="2" max="2" width="10.625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.875" style="3" customWidth="1"/>
+    <col min="6" max="8" width="8.875" style="3"/>
     <col min="9" max="9" width="14.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="12.375" style="2" customWidth="1"/>
     <col min="11" max="11" width="17.5" style="3" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="2"/>
-    <col min="14" max="16384" width="8.83203125" style="3"/>
+    <col min="12" max="12" width="16.625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="8.875" style="2"/>
+    <col min="14" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -4350,7 +4370,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="28"/>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B8" s="47" t="s">
         <v>210</v>
       </c>
@@ -4374,7 +4394,7 @@
       <c r="L8" s="7"/>
       <c r="M8" s="28"/>
     </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B9" s="50" t="s">
         <v>330</v>
       </c>
@@ -4400,7 +4420,7 @@
       </c>
       <c r="M9" s="28"/>
     </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B10" s="40"/>
       <c r="C10" s="40"/>
       <c r="D10" s="53" t="s">
@@ -4420,7 +4440,7 @@
       <c r="L10" s="7"/>
       <c r="M10" s="28"/>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B11" s="41" t="s">
         <v>220</v>
       </c>
@@ -4446,7 +4466,7 @@
       <c r="L11" s="7"/>
       <c r="M11" s="28"/>
     </row>
-    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B12" s="44" t="s">
         <v>224</v>
       </c>
@@ -4541,7 +4561,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="45" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" ht="42.75" x14ac:dyDescent="0.2">
       <c r="I18" s="4" t="s">
         <v>273</v>
       </c>
@@ -4554,7 +4574,7 @@
       <c r="L18" s="5"/>
       <c r="M18" s="36"/>
     </row>
-    <row r="19" spans="2:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B19" s="39" t="s">
         <v>239</v>
       </c>
@@ -4630,7 +4650,7 @@
       <c r="L21" s="7"/>
       <c r="M21" s="28"/>
     </row>
-    <row r="22" spans="2:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B22" s="47" t="s">
         <v>241</v>
       </c>
@@ -4656,7 +4676,7 @@
       <c r="L22" s="7"/>
       <c r="M22" s="28"/>
     </row>
-    <row r="23" spans="2:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B23" s="47" t="s">
         <v>242</v>
       </c>
@@ -4693,7 +4713,7 @@
       <c r="E24" s="51"/>
       <c r="F24" s="52"/>
     </row>
-    <row r="25" spans="2:13" ht="26" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B25" s="40"/>
       <c r="C25" s="40"/>
       <c r="D25" s="53" t="s">
@@ -4877,7 +4897,7 @@
       <c r="L36" s="23"/>
       <c r="M36" s="62"/>
     </row>
-    <row r="37" spans="2:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B37" s="6" t="s">
         <v>375</v>
       </c>
@@ -4903,7 +4923,7 @@
       </c>
       <c r="M37" s="62"/>
     </row>
-    <row r="38" spans="2:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B38" s="6" t="s">
         <v>377</v>
       </c>
@@ -4951,7 +4971,7 @@
       <c r="L39" s="64"/>
       <c r="M39" s="65"/>
     </row>
-    <row r="40" spans="2:13" ht="26" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="I40" s="55"/>
       <c r="J40" s="55"/>
       <c r="K40" s="66"/>
@@ -4986,7 +5006,7 @@
       </c>
       <c r="M42" s="55"/>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B43" s="16" t="s">
         <v>5</v>
       </c>
@@ -5016,7 +5036,7 @@
       </c>
       <c r="M43" s="55"/>
     </row>
-    <row r="44" spans="2:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:13" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="s">
         <v>406</v>
       </c>

</xml_diff>